<commit_message>
Added group 50433 to the initial dataset that Megan sent me - she may have excluded it for a reason, so it might come back out again
</commit_message>
<xml_diff>
--- a/sample_files/OVI_XrayGroup_Centers.xlsx
+++ b/sample_files/OVI_XrayGroup_Centers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donahue/Desktop/Projects/OVI_Groups/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dt237/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1176C3F-3621-FE4F-998D-F351D0096E85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03880EBE-3097-DF48-9256-081F1AE24D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{18E5B9BB-4EBB-9C4B-8748-11FCB6DBDBA9}"/>
   </bookViews>
@@ -92,9 +92,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09EB9D59-2939-0F44-92EB-AC49EE85C0C0}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -480,7 +479,7 @@
       <c r="B5">
         <v>0.13400000000000001</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>150.21492000000001</v>
       </c>
       <c r="D5">
@@ -494,10 +493,10 @@
       <c r="B6">
         <v>0.14499999999999999</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>129.49680000000001</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>44.248699999999999</v>
       </c>
     </row>
@@ -508,10 +507,10 @@
       <c r="B7">
         <v>0.127</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>230.11199999999999</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>28.88775</v>
       </c>
     </row>
@@ -522,11 +521,25 @@
       <c r="B8">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>328.76992000000001</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>-9.5888054999999994</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>50433</v>
+      </c>
+      <c r="B9">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C9">
+        <v>157.732</v>
+      </c>
+      <c r="D9">
+        <v>30.844000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made a small change to the coords of 50433, it didn't really represent where the X-ray emission and the galaxies are
</commit_message>
<xml_diff>
--- a/sample_files/OVI_XrayGroup_Centers.xlsx
+++ b/sample_files/OVI_XrayGroup_Centers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dt237/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03880EBE-3097-DF48-9256-081F1AE24D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4B86BC0-30F3-1846-BB65-52E8263309F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{18E5B9BB-4EBB-9C4B-8748-11FCB6DBDBA9}"/>
   </bookViews>
@@ -411,7 +411,7 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,10 +536,10 @@
         <v>0.13600000000000001</v>
       </c>
       <c r="C9">
-        <v>157.732</v>
+        <v>157.75800000000001</v>
       </c>
       <c r="D9">
-        <v>30.844000000000001</v>
+        <v>30.861999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>